<commit_message>
ajuste na agenda3.0 webhost, erro de cabeçalho e reportado no doc de testes
</commit_message>
<xml_diff>
--- a/phpbasico/agenda-nilo/3.0(000webhost)/stand/Doc_testes.xlsx
+++ b/phpbasico/agenda-nilo/3.0(000webhost)/stand/Doc_testes.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Senac\Uc5\phpbasico\agenda-nilo\3.0\stand\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\eduardo\Uc5\phpbasico\agenda-nilo\3.0(000webhost)\stand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2845B5CE-39BA-4891-BD6A-3C3688CB2125}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Banco dados" sheetId="1" r:id="rId1"/>
     <sheet name="Servidor" sheetId="2" r:id="rId2"/>
-    <sheet name="Navegadores" sheetId="3" r:id="rId3"/>
-    <sheet name="Dispositivos" sheetId="4" r:id="rId4"/>
-    <sheet name="Validaçoes" sheetId="5" r:id="rId5"/>
+    <sheet name="outros" sheetId="6" r:id="rId3"/>
+    <sheet name="Navegadores" sheetId="3" r:id="rId4"/>
+    <sheet name="Dispositivos" sheetId="4" r:id="rId5"/>
+    <sheet name="Validaçoes" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="59">
   <si>
     <t>tipo</t>
   </si>
@@ -160,12 +160,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>ftp.webcindario.com</t>
-  </si>
-  <si>
-    <t>agenda3edu-fer</t>
-  </si>
-  <si>
     <t>agenda123edu</t>
   </si>
   <si>
@@ -175,15 +169,6 @@
     <t>status</t>
   </si>
   <si>
-    <t>tive problema em conectar de primeira porque confundi com FTP do file zila, mas OK</t>
-  </si>
-  <si>
-    <t>mysql.webcindario.com</t>
-  </si>
-  <si>
-    <t>agenda3edu_fer</t>
-  </si>
-  <si>
     <t>Base de dados</t>
   </si>
   <si>
@@ -197,12 +182,36 @@
   </si>
   <si>
     <t>Ainda não tambem</t>
+  </si>
+  <si>
+    <t>agenda123</t>
+  </si>
+  <si>
+    <t>files.000webhost.com</t>
+  </si>
+  <si>
+    <t>agenda3-edu-fer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id10937667_agenda3edu_fer </t>
+  </si>
+  <si>
+    <t>id10937667_agenda3edu_fer</t>
+  </si>
+  <si>
+    <t>localhost</t>
+  </si>
+  <si>
+    <t>OBS</t>
+  </si>
+  <si>
+    <t>Erro de cabeçalho no validar, foi resolvido com adiçao de ob_star() antes de todo o codigo dentro do php e com ob_end_flush().</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -273,7 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -283,19 +292,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
@@ -306,19 +328,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="180"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -599,17 +614,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:K8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -621,7 +637,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -632,72 +648,70 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="10"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="10"/>
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="11"/>
+      <c r="C4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="10"/>
       <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="C5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="11"/>
+        <v>46</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="10"/>
       <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="11"/>
+      <c r="C7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="10"/>
       <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="10"/>
       <c r="B9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="6"/>
@@ -709,13 +723,12 @@
       <c r="J9" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
+    <mergeCell ref="A2:A9"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C8:K8"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A2:A9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -723,67 +736,70 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="10"/>
+      <c r="C2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="11"/>
       <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="11"/>
+      <c r="C3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="11"/>
       <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="11"/>
+      <c r="C4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="11"/>
       <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
+      <c r="C5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="11"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -794,18 +810,77 @@
     <mergeCell ref="C5:I5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{20398F43-300C-49A8-B0AC-3CF27ED456D5}"/>
+    <hyperlink ref="C2" r:id="rId1" display="ftp.webcindario.com"/>
   </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B4:D5"/>
+    <mergeCell ref="B6:D10"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4:R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,60 +902,60 @@
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12" t="s">
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12" t="s">
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12" t="s">
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12" t="s">
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12" t="s">
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="12"/>
-      <c r="AC2" s="12"/>
-      <c r="AD2" s="12" t="s">
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AE2" s="12"/>
-      <c r="AF2" s="12"/>
-      <c r="AG2" s="12"/>
+      <c r="AE2" s="15"/>
+      <c r="AF2" s="15"/>
+      <c r="AG2" s="15"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="11"/>
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -979,99 +1054,94 @@
       </c>
     </row>
     <row r="4" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="6"/>
-      <c r="R4" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="S4" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="T4" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="U4" s="18" t="s">
-        <v>54</v>
+      <c r="R4" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="T4" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="U4" s="13" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="18"/>
+      <c r="A5" s="11"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="13"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="20"/>
+      <c r="A6" s="11"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="7"/>
       <c r="W6" s="5"/>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="18"/>
+      <c r="A7" s="11"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="13"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="18"/>
+      <c r="A8" s="11"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="13"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="18"/>
+      <c r="A9" s="11"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="13"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="18"/>
+      <c r="A10" s="11"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="13"/>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="R11" s="16"/>
+      <c r="A11" s="11"/>
+      <c r="R11" s="17"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="R12" s="16"/>
+      <c r="A12" s="11"/>
+      <c r="R12" s="17"/>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="R13" s="16"/>
+      <c r="A13" s="11"/>
+      <c r="R13" s="17"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="R14" s="16"/>
+      <c r="A14" s="11"/>
+      <c r="R14" s="17"/>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="R15" s="16"/>
+      <c r="A15" s="11"/>
+      <c r="R15" s="17"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="R16" s="16"/>
+      <c r="A16" s="11"/>
+      <c r="R16" s="17"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
+      <c r="A17" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="U4:U10"/>
-    <mergeCell ref="S4:S10"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="T4:T10"/>
-    <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F2:I2"/>
@@ -1079,6 +1149,11 @@
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:U2"/>
     <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="U4:U10"/>
+    <mergeCell ref="S4:S10"/>
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="T4:T10"/>
+    <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="R4:R16"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1086,8 +1161,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1112,7 +1187,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B2" t="s">
@@ -1137,24 +1212,24 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
+      <c r="A3" s="18"/>
       <c r="B3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
+      <c r="A4" s="18"/>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="18"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+      <c r="A6" s="18"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -1177,8 +1252,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1188,31 +1263,31 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="12" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="10"/>
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -1222,26 +1297,26 @@
       <c r="D3" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="8" t="s">
+      <c r="F3" s="20"/>
+      <c r="G3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="8"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="10"/>
       <c r="B4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="10"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="10"/>
       <c r="L6" s="5"/>
     </row>
   </sheetData>

</xml_diff>